<commit_message>
2018-07-01 freezer and cohort 1
</commit_message>
<xml_diff>
--- a/Data/Storage/2018_storage_minus80_information.xlsx
+++ b/Data/Storage/2018_storage_minus80_information.xlsx
@@ -1,24 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hannahchu\Documents\GitHub\Proteome_stability_project\Data\Storage\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{189E1E6D-0244-4906-9B76-6C16578B0065}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="28705"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="8715" yWindow="465" windowWidth="38235" windowHeight="23325" activeTab="2" xr2:uid="{11D8066D-8F91-E240-B83C-274814A92F49}"/>
+    <workbookView xWindow="1020" yWindow="0" windowWidth="25360" windowHeight="14640" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Description" sheetId="3" r:id="rId1"/>
     <sheet name="R1_P1" sheetId="14" r:id="rId2"/>
     <sheet name="R3_P6" sheetId="2" r:id="rId3"/>
+    <sheet name="R3_P7" sheetId="15" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -27,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="40">
   <si>
     <t>Date</t>
   </si>
@@ -99,12 +97,60 @@
   </si>
   <si>
     <t>50uL p86 (1-5)</t>
+  </si>
+  <si>
+    <t>2018-07-01</t>
+  </si>
+  <si>
+    <t>DSPR Cohorts</t>
+  </si>
+  <si>
+    <t>R3_P7</t>
+  </si>
+  <si>
+    <t>vials with DSPR lines per cohort</t>
+  </si>
+  <si>
+    <t>C1A7</t>
+  </si>
+  <si>
+    <t>C1A2</t>
+  </si>
+  <si>
+    <t>C1B3</t>
+  </si>
+  <si>
+    <t>C1A5</t>
+  </si>
+  <si>
+    <t>C1A6</t>
+  </si>
+  <si>
+    <t>C1A4</t>
+  </si>
+  <si>
+    <t>C1A1</t>
+  </si>
+  <si>
+    <t>C1B6</t>
+  </si>
+  <si>
+    <t>C1B4</t>
+  </si>
+  <si>
+    <t>C1A3</t>
+  </si>
+  <si>
+    <t>C1B7</t>
+  </si>
+  <si>
+    <t>SURF NB#001 pg 92</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -154,16 +200,16 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -171,7 +217,7 @@
       <left/>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -180,7 +226,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -189,6 +235,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -251,7 +303,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -303,7 +355,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -497,88 +549,93 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62AA3223-7459-4543-B6A5-A6ABC614FE59}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="23.25" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="23" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="16384" width="10.875" style="4"/>
+    <col min="1" max="16384" width="10.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1">
       <c r="A1" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:1">
       <c r="A3" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:1">
       <c r="A4" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:1">
       <c r="A6" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:1">
       <c r="A7" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:1">
       <c r="A9" s="4" t="s">
         <v>13</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5546B438-9FC4-4E48-82EF-1ECCE0EBABA4}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L19"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="55" workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.375" defaultRowHeight="45.95" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="15.33203125" defaultRowHeight="46" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="26" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.375" style="2"/>
-    <col min="3" max="3" width="19.25" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" style="2"/>
+    <col min="3" max="3" width="19.1640625" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="21" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="15.375" style="2"/>
+    <col min="6" max="16384" width="15.33203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" ht="46" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" ht="46" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" ht="46" customHeight="1">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -586,22 +643,22 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" ht="46" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" ht="46" customHeight="1">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" ht="46" customHeight="1">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" ht="46" customHeight="1">
       <c r="B8" s="3"/>
       <c r="C8" s="3">
         <v>1</v>
@@ -634,7 +691,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" ht="46" customHeight="1">
       <c r="B9" s="3">
         <v>1</v>
       </c>
@@ -649,7 +706,7 @@
       <c r="K9" s="3"/>
       <c r="L9" s="3"/>
     </row>
-    <row r="10" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" ht="46" customHeight="1">
       <c r="B10" s="3">
         <v>2</v>
       </c>
@@ -664,7 +721,7 @@
       <c r="K10" s="3"/>
       <c r="L10" s="3"/>
     </row>
-    <row r="11" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" ht="46" customHeight="1">
       <c r="B11" s="3">
         <v>3</v>
       </c>
@@ -679,7 +736,7 @@
       <c r="K11" s="3"/>
       <c r="L11" s="3"/>
     </row>
-    <row r="12" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" ht="46" customHeight="1">
       <c r="B12" s="3">
         <v>4</v>
       </c>
@@ -694,7 +751,7 @@
       <c r="K12" s="3"/>
       <c r="L12" s="3"/>
     </row>
-    <row r="13" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" ht="46" customHeight="1">
       <c r="B13" s="3">
         <v>5</v>
       </c>
@@ -709,7 +766,7 @@
       <c r="K13" s="3"/>
       <c r="L13" s="3"/>
     </row>
-    <row r="14" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" ht="46" customHeight="1">
       <c r="B14" s="3">
         <v>6</v>
       </c>
@@ -724,7 +781,7 @@
       <c r="K14" s="3"/>
       <c r="L14" s="3"/>
     </row>
-    <row r="15" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" ht="46" customHeight="1">
       <c r="B15" s="3">
         <v>7</v>
       </c>
@@ -739,7 +796,7 @@
       <c r="K15" s="3"/>
       <c r="L15" s="3"/>
     </row>
-    <row r="16" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" ht="46" customHeight="1">
       <c r="B16" s="3">
         <v>8</v>
       </c>
@@ -754,7 +811,7 @@
       <c r="K16" s="3"/>
       <c r="L16" s="3"/>
     </row>
-    <row r="17" spans="2:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:12" ht="46" customHeight="1">
       <c r="B17" s="3">
         <v>9</v>
       </c>
@@ -769,7 +826,7 @@
       <c r="K17" s="3"/>
       <c r="L17" s="3"/>
     </row>
-    <row r="18" spans="2:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:12" ht="46" customHeight="1">
       <c r="B18" s="3">
         <v>10</v>
       </c>
@@ -784,7 +841,7 @@
       <c r="K18" s="3"/>
       <c r="L18" s="3"/>
     </row>
-    <row r="19" spans="2:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:12" ht="46" customHeight="1">
       <c r="B19" s="5" t="s">
         <v>6</v>
       </c>
@@ -805,29 +862,34 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5409961-BC8A-FB45-B43E-30E9D7F7D292}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView topLeftCell="A2" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="55" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.375" defaultRowHeight="45.95" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="15.33203125" defaultRowHeight="46" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="26" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.375" style="2"/>
-    <col min="3" max="3" width="19.25" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" style="2"/>
+    <col min="3" max="3" width="19.1640625" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="7" width="21" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="23.5" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="23.5" style="2" customWidth="1"/>
-    <col min="10" max="16384" width="15.375" style="2"/>
+    <col min="10" max="16384" width="15.33203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" ht="46" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -835,7 +897,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" ht="46" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -843,7 +905,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" ht="46" customHeight="1">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -851,12 +913,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" ht="46" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" ht="46" customHeight="1">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -864,7 +926,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" ht="46" customHeight="1">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
@@ -872,7 +934,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" ht="46" customHeight="1">
       <c r="B8" s="3"/>
       <c r="C8" s="3">
         <v>1</v>
@@ -905,7 +967,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" ht="46" customHeight="1">
       <c r="B9" s="3">
         <v>1</v>
       </c>
@@ -934,7 +996,7 @@
       <c r="K9" s="3"/>
       <c r="L9" s="3"/>
     </row>
-    <row r="10" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" ht="46" customHeight="1">
       <c r="B10" s="3">
         <v>2</v>
       </c>
@@ -949,7 +1011,7 @@
       <c r="K10" s="3"/>
       <c r="L10" s="3"/>
     </row>
-    <row r="11" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" ht="46" customHeight="1">
       <c r="B11" s="3">
         <v>3</v>
       </c>
@@ -964,7 +1026,7 @@
       <c r="K11" s="3"/>
       <c r="L11" s="3"/>
     </row>
-    <row r="12" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" ht="46" customHeight="1">
       <c r="B12" s="3">
         <v>4</v>
       </c>
@@ -979,7 +1041,7 @@
       <c r="K12" s="3"/>
       <c r="L12" s="3"/>
     </row>
-    <row r="13" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" ht="46" customHeight="1">
       <c r="B13" s="3">
         <v>5</v>
       </c>
@@ -994,7 +1056,7 @@
       <c r="K13" s="3"/>
       <c r="L13" s="3"/>
     </row>
-    <row r="14" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" ht="46" customHeight="1">
       <c r="B14" s="3">
         <v>6</v>
       </c>
@@ -1009,7 +1071,7 @@
       <c r="K14" s="3"/>
       <c r="L14" s="3"/>
     </row>
-    <row r="15" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" ht="46" customHeight="1">
       <c r="B15" s="3">
         <v>7</v>
       </c>
@@ -1024,7 +1086,7 @@
       <c r="K15" s="3"/>
       <c r="L15" s="3"/>
     </row>
-    <row r="16" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" ht="46" customHeight="1">
       <c r="B16" s="3">
         <v>8</v>
       </c>
@@ -1039,7 +1101,7 @@
       <c r="K16" s="3"/>
       <c r="L16" s="3"/>
     </row>
-    <row r="17" spans="2:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:12" ht="46" customHeight="1">
       <c r="B17" s="3">
         <v>9</v>
       </c>
@@ -1054,7 +1116,7 @@
       <c r="K17" s="3"/>
       <c r="L17" s="3"/>
     </row>
-    <row r="18" spans="2:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:12" ht="46" customHeight="1">
       <c r="B18" s="3">
         <v>10</v>
       </c>
@@ -1069,7 +1131,7 @@
       <c r="K18" s="3"/>
       <c r="L18" s="3"/>
     </row>
-    <row r="19" spans="2:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:12" ht="46" customHeight="1">
       <c r="B19" s="5" t="s">
         <v>6</v>
       </c>
@@ -1090,5 +1152,305 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="55" workbookViewId="0">
+      <selection activeCell="J5" activeCellId="1" sqref="B6 J5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="15.33203125" defaultRowHeight="46" customHeight="1" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="26" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" style="2"/>
+    <col min="3" max="3" width="19.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="21" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="15.33203125" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="46" customHeight="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="46" customHeight="1">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="46" customHeight="1">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="46" customHeight="1">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="46" customHeight="1">
+      <c r="A5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="46" customHeight="1">
+      <c r="A6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="46" customHeight="1">
+      <c r="B8" s="3"/>
+      <c r="C8" s="3">
+        <v>1</v>
+      </c>
+      <c r="D8" s="3">
+        <v>2</v>
+      </c>
+      <c r="E8" s="3">
+        <v>3</v>
+      </c>
+      <c r="F8" s="3">
+        <v>4</v>
+      </c>
+      <c r="G8" s="3">
+        <v>5</v>
+      </c>
+      <c r="H8" s="3">
+        <v>6</v>
+      </c>
+      <c r="I8" s="3">
+        <v>7</v>
+      </c>
+      <c r="J8" s="3">
+        <v>8</v>
+      </c>
+      <c r="K8" s="3">
+        <v>9</v>
+      </c>
+      <c r="L8" s="7"/>
+    </row>
+    <row r="9" spans="1:12" ht="46" customHeight="1">
+      <c r="B9" s="3">
+        <v>1</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="K9" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="L9" s="7"/>
+    </row>
+    <row r="10" spans="1:12" ht="46" customHeight="1">
+      <c r="B10" s="3">
+        <v>2</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="7"/>
+    </row>
+    <row r="11" spans="1:12" ht="46" customHeight="1">
+      <c r="B11" s="3">
+        <v>3</v>
+      </c>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="7"/>
+    </row>
+    <row r="12" spans="1:12" ht="46" customHeight="1">
+      <c r="B12" s="3">
+        <v>4</v>
+      </c>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="7"/>
+    </row>
+    <row r="13" spans="1:12" ht="46" customHeight="1">
+      <c r="B13" s="3">
+        <v>5</v>
+      </c>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="7"/>
+    </row>
+    <row r="14" spans="1:12" ht="46" customHeight="1">
+      <c r="B14" s="3">
+        <v>6</v>
+      </c>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="7"/>
+    </row>
+    <row r="15" spans="1:12" ht="46" customHeight="1">
+      <c r="B15" s="3">
+        <v>7</v>
+      </c>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="7"/>
+    </row>
+    <row r="16" spans="1:12" ht="46" customHeight="1">
+      <c r="B16" s="3">
+        <v>8</v>
+      </c>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="3"/>
+      <c r="L16" s="7"/>
+    </row>
+    <row r="17" spans="2:12" ht="46" customHeight="1">
+      <c r="B17" s="3">
+        <v>9</v>
+      </c>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="3"/>
+      <c r="L17" s="7"/>
+    </row>
+    <row r="18" spans="2:12" ht="46" customHeight="1">
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="7"/>
+      <c r="I18" s="7"/>
+      <c r="J18" s="7"/>
+      <c r="K18" s="7"/>
+      <c r="L18" s="7"/>
+    </row>
+    <row r="19" spans="2:12" ht="46" customHeight="1">
+      <c r="B19" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="6"/>
+      <c r="J19" s="6"/>
+      <c r="K19" s="6"/>
+      <c r="L19" s="6"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B19:L19"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>